<commit_message>
Added embodied emission params from transportation/greet_model
</commit_message>
<xml_diff>
--- a/model_constraints/trn_constraints_baseline.xlsx
+++ b/model_constraints/trn_constraints_baseline.xlsx
@@ -6520,7 +6520,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6543,7 +6543,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6562,11 +6562,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.875032334</v>
+        <v>2.344622521</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6585,11 +6585,11 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.033787219</v>
+        <v>2.344622521</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6608,11 +6608,11 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2.344622521</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6631,11 +6631,11 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2.344622521</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=96.504725252, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6658,7 +6658,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6681,7 +6681,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6700,11 +6700,11 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2.085179165</v>
+        <v>2.425110906</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6723,11 +6723,11 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1.344823905</v>
+        <v>2.425110906</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6746,11 +6746,11 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2.425110906</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6769,11 +6769,11 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2.425110906</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=62.314639545, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6796,7 +6796,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6819,7 +6819,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6838,11 +6838,11 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2.106987557</v>
+        <v>2.432917599</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6861,11 +6861,11 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.382321358</v>
+        <v>2.432917599</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6884,11 +6884,11 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>2.432917599</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6907,11 +6907,11 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2.432917599</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=59.087369747, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6934,7 +6934,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6957,7 +6957,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6976,11 +6976,11 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2.358546837</v>
+        <v>2.516605919</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -6999,11 +6999,11 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1.909561872</v>
+        <v>2.516605919</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7022,11 +7022,11 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1.079304988</v>
+        <v>2.516605919</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7045,11 +7045,11 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>2.516605919</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=25.422725313, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7072,7 +7072,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7095,7 +7095,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7114,11 +7114,11 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.542625677</v>
+        <v>2.571370438</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7137,11 +7137,11 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2.443938781</v>
+        <v>2.571370438</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7160,11 +7160,11 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2.138233966</v>
+        <v>2.571370438</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7183,11 +7183,11 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.438031182</v>
+        <v>2.571370438</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7210,7 +7210,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7252,11 +7252,11 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2.542625677</v>
+        <v>2.571370438</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7275,11 +7275,11 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.443938781</v>
+        <v>2.571370438</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7298,11 +7298,11 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2.138233966</v>
+        <v>2.571370438</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7321,11 +7321,11 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.438031182</v>
+        <v>2.571370438</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.272708968, emergence_rate=0.290746047, saturation=7514.810858897)</t>
         </is>
       </c>
     </row>
@@ -7348,7 +7348,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7371,7 +7371,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7390,11 +7390,11 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2.317999179</v>
+        <v>2.50385326</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7413,11 +7413,11 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1.810993544</v>
+        <v>2.50385326</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7436,11 +7436,11 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>2.50385326</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7459,11 +7459,11 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>2.50385326</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=9.246201158, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7509,7 +7509,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7528,11 +7528,11 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2.537432075</v>
+        <v>2.569891385</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7551,11 +7551,11 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.426602377</v>
+        <v>2.569891385</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7574,11 +7574,11 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.089325108</v>
+        <v>2.569891385</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7597,11 +7597,11 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1.351867306</v>
+        <v>2.569891385</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.468433178, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7647,7 +7647,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7666,11 +7666,11 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2.547152184</v>
+        <v>2.572656546</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7689,11 +7689,11 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2.459169712</v>
+        <v>2.572656546</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7712,11 +7712,11 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2.182318833</v>
+        <v>2.572656546</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7735,11 +7735,11 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>1.520844638</v>
+        <v>2.572656546</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7762,7 +7762,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7804,11 +7804,11 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>2.547152184</v>
+        <v>2.572656546</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7827,11 +7827,11 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>2.459169712</v>
+        <v>2.572656546</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7850,11 +7850,11 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>2.182318833</v>
+        <v>2.572656546</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7873,11 +7873,11 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1.520844638</v>
+        <v>2.572656546</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7923,7 +7923,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7942,11 +7942,11 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>2.547152184</v>
+        <v>2.572656546</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7965,11 +7965,11 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2.459169712</v>
+        <v>2.572656546</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -7988,11 +7988,11 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>2.182318833</v>
+        <v>2.572656546</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -8011,11 +8011,11 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>1.520844638</v>
+        <v>2.572656546</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=1.149195195, emergence_rate=0.290746047, saturation=2282.233573246)</t>
         </is>
       </c>
     </row>
@@ -8038,7 +8038,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8061,7 +8061,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8080,11 +8080,11 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>2.53242352</v>
+        <v>2.568461567</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8103,11 +8103,11 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>2.410023118</v>
+        <v>2.568461567</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8126,11 +8126,11 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>2.043776302</v>
+        <v>2.568461567</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8149,11 +8149,11 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>1.2765995</v>
+        <v>2.568461567</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8176,7 +8176,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8199,7 +8199,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8218,11 +8218,11 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>2.53242352</v>
+        <v>2.568461567</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8241,11 +8241,11 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>2.410023118</v>
+        <v>2.568461567</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8264,11 +8264,11 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>2.043776302</v>
+        <v>2.568461567</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8287,11 +8287,11 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>1.2765995</v>
+        <v>2.568461567</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8314,7 +8314,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8337,7 +8337,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8356,11 +8356,11 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>2.53242352</v>
+        <v>2.568461567</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8379,11 +8379,11 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>2.410023118</v>
+        <v>2.568461567</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8402,11 +8402,11 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2.043776302</v>
+        <v>2.568461567</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8425,11 +8425,11 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>1.2765995</v>
+        <v>2.568461567</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8452,7 +8452,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8475,7 +8475,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8494,11 +8494,11 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>2.53242352</v>
+        <v>2.568461567</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8517,11 +8517,11 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>2.410023118</v>
+        <v>2.568461567</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8540,11 +8540,11 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>2.043776302</v>
+        <v>2.568461567</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8563,11 +8563,11 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>1.2765995</v>
+        <v>2.568461567</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.150530587, emergence_rate=0.290746047, saturation=210.286535431)</t>
         </is>
       </c>
     </row>
@@ -8590,7 +8590,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8613,7 +8613,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8632,11 +8632,11 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>2.539337798</v>
+        <v>2.570434527</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8655,11 +8655,11 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>2.432946555</v>
+        <v>2.570434527</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8678,11 +8678,11 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>2.107068945</v>
+        <v>2.570434527</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8701,11 +8701,11 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>1.382463389</v>
+        <v>2.570434527</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8728,7 +8728,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8770,11 +8770,11 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>2.539337798</v>
+        <v>2.570434527</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8793,11 +8793,11 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>2.432946555</v>
+        <v>2.570434527</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8816,11 +8816,11 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>2.107068945</v>
+        <v>2.570434527</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8839,11 +8839,11 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>1.382463389</v>
+        <v>2.570434527</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8866,7 +8866,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8889,7 +8889,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8908,11 +8908,11 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>2.539337798</v>
+        <v>2.570434527</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8931,11 +8931,11 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>2.432946555</v>
+        <v>2.570434527</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8954,11 +8954,11 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>2.107068945</v>
+        <v>2.570434527</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -8977,11 +8977,11 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>1.382463389</v>
+        <v>2.570434527</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9004,7 +9004,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9027,7 +9027,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9046,11 +9046,11 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>2.539337798</v>
+        <v>2.570434527</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9069,11 +9069,11 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>2.432946555</v>
+        <v>2.570434527</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9092,11 +9092,11 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>2.107068945</v>
+        <v>2.570434527</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9115,11 +9115,11 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>1.382463389</v>
+        <v>2.570434527</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=0.421728299, emergence_rate=0.290746047, saturation=684.705896655)</t>
         </is>
       </c>
     </row>
@@ -9142,7 +9142,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9165,7 +9165,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9184,11 +9184,11 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>2.035900162</v>
+        <v>2.407112434</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9207,11 +9207,11 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>1.264042725</v>
+        <v>2.407112434</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9230,11 +9230,11 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>2.407112434</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9253,11 +9253,11 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>2.407112434</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=75.36582092, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9280,7 +9280,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9303,7 +9303,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9322,11 +9322,11 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>2.492725572</v>
+        <v>2.557006978</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9345,11 +9345,11 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>2.283295321</v>
+        <v>2.557006978</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9368,11 +9368,11 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>1.731241426</v>
+        <v>2.557006978</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9391,11 +9391,11 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>1</v>
+        <v>2.557006978</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=10.53101724, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9418,7 +9418,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9441,7 +9441,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9460,11 +9460,11 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>2.544007011</v>
+        <v>2.571763206</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9483,11 +9483,11 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>2.448574702</v>
+        <v>2.571763206</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9506,11 +9506,11 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>2.151540183</v>
+        <v>2.571763206</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9529,11 +9529,11 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>1.462493329</v>
+        <v>2.571763206</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.451344823, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9556,7 +9556,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9579,7 +9579,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9598,11 +9598,11 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>2.546915659</v>
+        <v>2.572589411</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9621,11 +9621,11 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>2.458371028</v>
+        <v>2.572589411</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9644,11 +9644,11 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>2.179980607</v>
+        <v>2.572589411</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9667,11 +9667,11 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>1.516322891</v>
+        <v>2.572589411</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9694,7 +9694,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9717,7 +9717,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9736,11 +9736,11 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>2.546915659</v>
+        <v>2.572589411</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9759,11 +9759,11 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>2.458371028</v>
+        <v>2.572589411</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9782,11 +9782,11 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>2.179980607</v>
+        <v>2.572589411</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>
@@ -9805,11 +9805,11 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>1.516322891</v>
+        <v>2.572589411</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Derived from projected net capacity simulated with a logistic diffusion model; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
+          <t>Derived from projected net capacity simulated with a logistic diffusion model, 5-year growth is frozen before first drop in projections; Median growth scenario (where initial_cap=4.112463111, emergence_rate=0.290746047, saturation=8112.435883697)</t>
         </is>
       </c>
     </row>

</xml_diff>